<commit_message>
Code Refactor as per Sonarlint
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/TestInput.xlsx
+++ b/src/test/resources/excel/TestInput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laksh\git\selenium-AFW\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058FE026-D184-4686-8331-267D3A52B928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA89C35-9741-4751-95C9-99FAF9EF8A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{95E5B64E-F434-4F35-8E70-B90CC0CDD42B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="34">
   <si>
     <t>UserName</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>MicrosoftEdge</t>
+  </si>
+  <si>
+    <t>Amazon.com: Computers &amp; Accessories: Electronics: Computer Accessories &amp; Peripherals, T3ablet Accessories &amp; More</t>
+  </si>
+  <si>
+    <t>Amazon.com: Computers &amp; Accessories: Electronics: Co-mputer Accessories &amp; Peripherals, Tablet Accessories &amp; More</t>
   </si>
 </sst>
 </file>
@@ -513,17 +519,17 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -537,7 +543,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -551,7 +557,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -565,7 +571,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>26</v>
       </c>
@@ -579,7 +585,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
@@ -606,20 +612,20 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -648,7 +654,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -677,7 +683,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -706,7 +712,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -735,7 +741,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
@@ -761,10 +767,10 @@
         <v>25</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
@@ -789,7 +795,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -815,10 +821,10 @@
         <v>25</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
@@ -847,7 +853,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Included selenoid and added github actions
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/TestInput.xlsx
+++ b/src/test/resources/excel/TestInput.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laksh\git\selenium-AFW\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA89C35-9741-4751-95C9-99FAF9EF8A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85FA4484-1164-4746-AC14-168F271B1A11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{95E5B64E-F434-4F35-8E70-B90CC0CDD42B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{95E5B64E-F434-4F35-8E70-B90CC0CDD42B}"/>
   </bookViews>
   <sheets>
     <sheet name="RunManager" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="35">
   <si>
     <t>UserName</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>Amazon.com: Computers &amp; Accessories: Electronics: Co-mputer Accessories &amp; Peripherals, Tablet Accessories &amp; More</t>
+  </si>
+  <si>
+    <t>84.0</t>
   </si>
 </sst>
 </file>
@@ -606,10 +609,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E9E4029-3958-4C69-854D-2D54083BF57F}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -717,7 +720,7 @@
         <v>26</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>17</v>
@@ -746,7 +749,7 @@
         <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>18</v>
@@ -775,7 +778,7 @@
         <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>31</v>
@@ -800,7 +803,7 @@
         <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>17</v>
@@ -829,7 +832,7 @@
         <v>27</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>18</v>
@@ -858,7 +861,7 @@
         <v>27</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>31</v>
@@ -879,6 +882,64 @@
         <v>25</v>
       </c>
       <c r="I9" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Git hub action changes - T1
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/TestInput.xlsx
+++ b/src/test/resources/excel/TestInput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laksh\git\selenium-AFW\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85FA4484-1164-4746-AC14-168F271B1A11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3375512E-B135-43DF-95F1-045C31715165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{95E5B64E-F434-4F35-8E70-B90CC0CDD42B}"/>
   </bookViews>
@@ -141,7 +141,7 @@
     <t>Amazon.com: Computers &amp; Accessories: Electronics: Co-mputer Accessories &amp; Peripherals, Tablet Accessories &amp; More</t>
   </si>
   <si>
-    <t>84.0</t>
+    <t>108.8</t>
   </si>
 </sst>
 </file>
@@ -612,7 +612,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Git hub action changes - T2
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/TestInput.xlsx
+++ b/src/test/resources/excel/TestInput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laksh\git\selenium-AFW\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3375512E-B135-43DF-95F1-045C31715165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA5B900-5B05-4563-B168-610C2D59AA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{95E5B64E-F434-4F35-8E70-B90CC0CDD42B}"/>
   </bookViews>
@@ -141,7 +141,7 @@
     <t>Amazon.com: Computers &amp; Accessories: Electronics: Co-mputer Accessories &amp; Peripherals, Tablet Accessories &amp; More</t>
   </si>
   <si>
-    <t>108.8</t>
+    <t>84.0</t>
   </si>
 </sst>
 </file>

</xml_diff>